<commit_message>
Adicionamos os evercícios dos módulos 'Primeiros passos para desenvolvimento web', 'Introdução a criação de websites com HTML5 e CSS3' e seus respectivos certificados.
</commit_message>
<xml_diff>
--- a/Evolução.xlsx
+++ b/Evolução.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\DIO\BOOTCAMP CARREFOUR WEB DEVELOPER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Workspace\DIO\BOOTCAMP CARREFOUR WEB DEVELOPER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73D0EEA-B075-41FB-8AE1-D61C1F63870D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85C1EAE-061C-4DC4-8693-521F0FC52628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Dia</t>
   </si>
@@ -70,7 +70,31 @@
     <t>Módulo</t>
   </si>
   <si>
-    <t>MODULO I</t>
+    <t>Primeiros passos para Desenvolvimento Web</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Introdução a criação de sites com HTML5 e CSS3</t>
+  </si>
+  <si>
+    <t>Construindo páginas para internet usando Bootstrap</t>
+  </si>
+  <si>
+    <t>Recriando a Interface do Netflix</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -197,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -232,17 +256,26 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C38" sqref="C37:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,21 +586,21 @@
         <v>2</v>
       </c>
       <c r="G1" s="11">
-        <f>SUM(D2:D50)</f>
-        <v>17</v>
+        <f>SUM(D2:D41)</f>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44669</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>11</v>
+      <c r="B2" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="12">
         <v>1</v>
       </c>
     </row>
@@ -575,11 +608,11 @@
       <c r="A3" s="3">
         <v>44670</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="12">
         <v>2</v>
       </c>
     </row>
@@ -587,11 +620,11 @@
       <c r="A4" s="3">
         <v>44670</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="12">
         <v>2</v>
       </c>
     </row>
@@ -599,11 +632,11 @@
       <c r="A5" s="3">
         <v>44671</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>4</v>
       </c>
     </row>
@@ -611,11 +644,11 @@
       <c r="A6" s="3">
         <v>44672</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>5</v>
       </c>
     </row>
@@ -623,333 +656,299 @@
       <c r="A7" s="3">
         <v>44673</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>44674</v>
-      </c>
-      <c r="B8" s="14"/>
+        <v>44673</v>
+      </c>
+      <c r="B8" s="18"/>
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>44675</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="4"/>
+        <v>44676</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>44676</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="8"/>
+        <v>44677</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>44677</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="8"/>
+        <v>44678</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>44678</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="8"/>
+        <v>44679</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>44679</v>
-      </c>
-      <c r="B13" s="3"/>
+        <v>44680</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>44680</v>
-      </c>
-      <c r="B14" s="3"/>
+        <v>44681</v>
+      </c>
+      <c r="B14" s="14"/>
       <c r="C14" s="8"/>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>44681</v>
-      </c>
-      <c r="B15" s="3"/>
+        <v>44682</v>
+      </c>
+      <c r="B15" s="14"/>
       <c r="C15" s="8"/>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>44682</v>
-      </c>
-      <c r="B16" s="3"/>
+        <v>44683</v>
+      </c>
+      <c r="B16" s="14"/>
       <c r="C16" s="8"/>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>44683</v>
-      </c>
-      <c r="B17" s="3"/>
+        <v>44684</v>
+      </c>
+      <c r="B17" s="14"/>
       <c r="C17" s="8"/>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>44684</v>
-      </c>
-      <c r="B18" s="3"/>
+        <v>44685</v>
+      </c>
+      <c r="B18" s="14"/>
       <c r="C18" s="8"/>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>44685</v>
-      </c>
-      <c r="B19" s="3"/>
+        <v>44686</v>
+      </c>
+      <c r="B19" s="14"/>
       <c r="C19" s="8"/>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>44686</v>
-      </c>
-      <c r="B20" s="3"/>
+        <v>44687</v>
+      </c>
+      <c r="B20" s="15"/>
       <c r="C20" s="8"/>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>44687</v>
-      </c>
-      <c r="B21" s="3"/>
+        <v>44688</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>18</v>
+      </c>
       <c r="C21" s="8"/>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>44688</v>
-      </c>
-      <c r="B22" s="3"/>
+        <v>44689</v>
+      </c>
+      <c r="B22" s="14"/>
       <c r="C22" s="8"/>
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>44689</v>
-      </c>
-      <c r="B23" s="3"/>
+        <v>44690</v>
+      </c>
+      <c r="B23" s="14"/>
       <c r="C23" s="8"/>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>44690</v>
-      </c>
-      <c r="B24" s="3"/>
+        <v>44691</v>
+      </c>
+      <c r="B24" s="14"/>
       <c r="C24" s="8"/>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>44691</v>
-      </c>
-      <c r="B25" s="3"/>
+        <v>44692</v>
+      </c>
+      <c r="B25" s="14"/>
       <c r="C25" s="8"/>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>44692</v>
-      </c>
-      <c r="B26" s="3"/>
+        <v>44693</v>
+      </c>
+      <c r="B26" s="15"/>
       <c r="C26" s="8"/>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>44693</v>
-      </c>
-      <c r="B27" s="3"/>
+        <v>44694</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>19</v>
+      </c>
       <c r="C27" s="8"/>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>44694</v>
-      </c>
-      <c r="B28" s="3"/>
+        <v>44695</v>
+      </c>
+      <c r="B28" s="14"/>
       <c r="C28" s="8"/>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>44695</v>
-      </c>
-      <c r="B29" s="3"/>
+        <v>44696</v>
+      </c>
+      <c r="B29" s="14"/>
       <c r="C29" s="8"/>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>44696</v>
-      </c>
-      <c r="B30" s="3"/>
+        <v>44697</v>
+      </c>
+      <c r="B30" s="14"/>
       <c r="C30" s="8"/>
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>44697</v>
-      </c>
-      <c r="B31" s="3"/>
+        <v>44698</v>
+      </c>
+      <c r="B31" s="14"/>
       <c r="C31" s="8"/>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>44698</v>
-      </c>
-      <c r="B32" s="3"/>
+        <v>44699</v>
+      </c>
+      <c r="B32" s="14"/>
       <c r="C32" s="8"/>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>44699</v>
-      </c>
-      <c r="B33" s="3"/>
+        <v>44700</v>
+      </c>
+      <c r="B33" s="14"/>
       <c r="C33" s="8"/>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>44700</v>
-      </c>
-      <c r="B34" s="3"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="8"/>
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="8"/>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="8"/>
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="14"/>
       <c r="C37" s="8"/>
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="14"/>
       <c r="C38" s="8"/>
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="B39" s="14"/>
       <c r="C39" s="8"/>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="B40" s="14"/>
       <c r="C40" s="8"/>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="B41" s="15"/>
       <c r="C41" s="8"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="4"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
+    <mergeCell ref="B27:B41"/>
     <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B13:B20"/>
+    <mergeCell ref="B21:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adicionamos o projeto do módulo 'Construindo páginas para internet com bootstrap' e seu respectivo certificado.
</commit_message>
<xml_diff>
--- a/Evolução.xlsx
+++ b/Evolução.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Workspace\DIO\BOOTCAMP CARREFOUR WEB DEVELOPER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85C1EAE-061C-4DC4-8693-521F0FC52628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB505F5-43CF-4069-8F3C-9971861839F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -560,7 +560,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C37:C38"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,7 +587,7 @@
       </c>
       <c r="G1" s="11">
         <f>SUM(D2:D41)</f>
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -698,7 +698,9 @@
       <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -708,7 +710,9 @@
       <c r="C11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">

</xml_diff>

<commit_message>
Adicionamos o projeto do módulo 'Recriando a Interface do Netflix' e atualizamos o arquivo de evolução.
</commit_message>
<xml_diff>
--- a/Evolução.xlsx
+++ b/Evolução.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Workspace\DIO\BOOTCAMP CARREFOUR WEB DEVELOPER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB505F5-43CF-4069-8F3C-9971861839F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889246BC-47F0-4D76-A866-3A0A99ED11F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Dia</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>Tema</t>
   </si>
 </sst>
 </file>
@@ -221,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -237,9 +240,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -559,48 +559,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.5703125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="6"/>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="11">
+      <c r="G1" s="10">
         <f>SUM(D2:D41)</f>
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44669</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>1</v>
       </c>
     </row>
@@ -608,11 +609,11 @@
       <c r="A3" s="3">
         <v>44670</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>2</v>
       </c>
     </row>
@@ -620,11 +621,11 @@
       <c r="A4" s="3">
         <v>44670</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>2</v>
       </c>
     </row>
@@ -632,11 +633,11 @@
       <c r="A5" s="3">
         <v>44671</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>4</v>
       </c>
     </row>
@@ -644,11 +645,11 @@
       <c r="A6" s="3">
         <v>44672</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>5</v>
       </c>
     </row>
@@ -656,11 +657,11 @@
       <c r="A7" s="3">
         <v>44673</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>2</v>
       </c>
     </row>
@@ -668,11 +669,11 @@
       <c r="A8" s="3">
         <v>44673</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>1</v>
       </c>
     </row>
@@ -680,13 +681,13 @@
       <c r="A9" s="3">
         <v>44676</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>6</v>
       </c>
     </row>
@@ -694,11 +695,11 @@
       <c r="A10" s="3">
         <v>44677</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="8" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <v>6</v>
       </c>
     </row>
@@ -706,11 +707,11 @@
       <c r="A11" s="3">
         <v>44678</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>4</v>
       </c>
     </row>
@@ -718,232 +719,234 @@
       <c r="A12" s="3">
         <v>44679</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="8" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="11">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44680</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44681</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44682</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="8"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="7"/>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44683</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="8"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="7"/>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>44684</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>44685</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="8"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="7"/>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>44686</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="8"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="7"/>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>44687</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="8"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="7"/>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>44688</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="7"/>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>44689</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="8"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>44690</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="8"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="7"/>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>44691</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="8"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="7"/>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>44692</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="8"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="7"/>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>44693</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="8"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="7"/>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>44694</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="8"/>
+      <c r="C27" s="7"/>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>44695</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="8"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="7"/>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>44696</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="8"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>44697</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="8"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="7"/>
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>44698</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="8"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="7"/>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>44699</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="8"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="7"/>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>44700</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="8"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="7"/>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="8"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="7"/>
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="8"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="7"/>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="8"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="7"/>
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="8"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="7"/>
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="8"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="7"/>
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="8"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="7"/>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="8"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="7"/>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="8"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="7"/>
       <c r="D41" s="4"/>
     </row>
   </sheetData>

</xml_diff>